<commit_message>
Correct an Index Bug, but should update the initial value of the reference codes as in the template
</commit_message>
<xml_diff>
--- a/Reference_codes.xlsx
+++ b/Reference_codes.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_3F4CD84F42A7590CC08E50FE16C0510BA3EAFB9A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4EBC2488-F06D-484F-9846-8C4C906D1248}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="22260" windowHeight="12640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ref_labels</t>
   </si>
@@ -46,18 +47,29 @@
   </si>
   <si>
     <t>cyb</t>
+  </si>
+  <si>
+    <t>Initial_value</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -85,7 +97,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -362,19 +374,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -384,8 +398,11 @@
       <c r="C1" t="s">
         <v>5</v>
       </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -395,8 +412,11 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
+      <c r="D2">
+        <v>4278.04</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -406,8 +426,11 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
+      <c r="D3">
+        <v>3170.73</v>
+      </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -417,8 +440,12 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
+      <c r="D4">
+        <v>1268.4100000000001</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>